<commit_message>
reviewed university names, get_virtual_events()
</commit_message>
<xml_diff>
--- a/docs/trends_paper/us_issues.xlsx
+++ b/docs/trends_paper/us_issues.xlsx
@@ -407,7 +407,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>404</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C14">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15">
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="C15">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="C16">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17">
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="C19">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="C20">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="C21">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="C24">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="C29">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="30">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="C34">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="35">
@@ -887,7 +887,7 @@
         </is>
       </c>
       <c r="C35">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="C36">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="37">
@@ -947,7 +947,7 @@
         </is>
       </c>
       <c r="C39">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40">
@@ -1067,7 +1067,7 @@
         </is>
       </c>
       <c r="C47">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="C49">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="C54">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55">
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="C55">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="56">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="C57">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="58">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="C58">
-        <v>1347</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="59">
@@ -1247,7 +1247,7 @@
         </is>
       </c>
       <c r="C59">
-        <v>510</v>
+        <v>533</v>
       </c>
     </row>
     <row r="60">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="C62">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="63">
@@ -1307,7 +1307,7 @@
         </is>
       </c>
       <c r="C63">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1353,17 +1353,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>39.56% (1,766)</t>
+          <t>39.79% (1,793)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30.17% (1,347)</t>
+          <t>30.03% (1,353)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11.42% (510)</t>
+          <t>11.83% (533)</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37.59% (1,678)</t>
+          <t>37.79% (1,703)</t>
         </is>
       </c>
     </row>
@@ -1387,12 +1387,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16.35% (730)</t>
+          <t>16.27% (733)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16.35% (730)</t>
+          <t>16.27% (733)</t>
         </is>
       </c>
     </row>
@@ -1404,12 +1404,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12.43% (555)</t>
+          <t>12.36% (557)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12.43% (555)</t>
+          <t>12.36% (557)</t>
         </is>
       </c>
     </row>
@@ -1421,12 +1421,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12.41% (554)</t>
+          <t>12.32% (555)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>12.41% (554)</t>
+          <t>12.32% (555)</t>
         </is>
       </c>
     </row>
@@ -1438,17 +1438,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10.19% (455)</t>
+          <t>10.14% (457)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7.97% (356)</t>
+          <t>7.92% (357)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2.44% (109)</t>
+          <t>2.44% (110)</t>
         </is>
       </c>
     </row>
@@ -1460,12 +1460,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10.15% (453)</t>
+          <t>10.08% (454)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10.15% (453)</t>
+          <t>10.08% (454)</t>
         </is>
       </c>
     </row>
@@ -1477,12 +1477,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9.05% (404)</t>
+          <t>9.41% (424)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>9.05% (404)</t>
+          <t>9.41% (424)</t>
         </is>
       </c>
     </row>
@@ -1494,12 +1494,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7.68% (343)</t>
+          <t>7.66% (345)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7.68% (343)</t>
+          <t>7.66% (345)</t>
         </is>
       </c>
     </row>
@@ -1511,12 +1511,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>6.63% (296)</t>
+          <t>6.61% (298)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>6.63% (296)</t>
+          <t>6.61% (298)</t>
         </is>
       </c>
     </row>
@@ -1528,12 +1528,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5.94% (265)</t>
+          <t>5.9% (266)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5.94% (265)</t>
+          <t>5.9% (266)</t>
         </is>
       </c>
     </row>
@@ -1545,12 +1545,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5% (223)</t>
+          <t>4.99% (225)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5% (223)</t>
+          <t>4.99% (225)</t>
         </is>
       </c>
     </row>
@@ -1562,12 +1562,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4.91% (219)</t>
+          <t>4.9% (221)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4.91% (219)</t>
+          <t>4.9% (221)</t>
         </is>
       </c>
     </row>
@@ -1579,12 +1579,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4.48% (200)</t>
+          <t>4.46% (201)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4.48% (200)</t>
+          <t>4.46% (201)</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1.19% (53)</t>
+          <t>1.18% (53)</t>
         </is>
       </c>
     </row>

</xml_diff>